<commit_message>
Bumpers & Body Mounts Release
</commit_message>
<xml_diff>
--- a/SOLIDWORKS 2019 FILES/BOM/DIFFERENTIAL-ASSY-BOM.xlsx
+++ b/SOLIDWORKS 2019 FILES/BOM/DIFFERENTIAL-ASSY-BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Google_Drive\GitHub\Rigid3D-Anka-RC-Short-Course-Truck\SOLIDWORKS 2019 FILES\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{101042EB-3EBC-4643-BB7D-FFA53F80BF30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{247EF8A7-2491-4D8F-A20F-A7D797194719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4155" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{A8AE94DA-4747-455A-8E90-B722CADEF95C}"/>
   </bookViews>
@@ -639,13 +639,8 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{6ADA6CAB-195B-4B3E-86F9-5026547BE4B6}" diskRevisions="1" revisionId="6" version="2">
-  <header guid="{0181FF28-EDB5-4795-A9C8-9F55187B6806}" dateTime="2022-05-28T03:56:24" maxSheetId="2" userName="Mehmet Sutaş" r:id="rId1">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{6ADA6CAB-195B-4B3E-86F9-5026547BE4B6}" dateTime="2022-05-28T13:27:40" maxSheetId="2" userName="Mehmet Sutaş" r:id="rId2" minRId="1" maxRId="6">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{648B0F46-6F6A-4783-BDAC-C8F647AEB9F2}" diskRevisions="1" revisionId="7" version="3">
+  <header guid="{648B0F46-6F6A-4783-BDAC-C8F647AEB9F2}" dateTime="2022-11-23T15:40:04" maxSheetId="2" userName="Mehmet Sutaş" r:id="rId3" minRId="7">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -653,390 +648,16 @@
 </headers>
 </file>
 
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
-</file>
-
-<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rrc rId="1" sId="1" ref="F1:F1048576" action="insertCol"/>
-  <rm rId="2" sheetId="1" source="D1:D1048576" destination="F1:F1048576" sourceSheetId="1">
-    <rfmt sheetId="1" xfDxf="1" sqref="F1:F1048576" start="0" length="0"/>
-    <rfmt sheetId="1" sqref="F1" start="0" length="0">
-      <dxf>
-        <font>
-          <sz val="12"/>
-          <color theme="1"/>
-          <name val="Century Gothic"/>
-          <family val="2"/>
-          <charset val="162"/>
-          <scheme val="none"/>
-        </font>
-        <alignment horizontal="center" vertical="center" wrapText="1"/>
-      </dxf>
-    </rfmt>
-    <rfmt sheetId="1" sqref="F2" start="0" length="0">
-      <dxf>
-        <font>
-          <sz val="12"/>
-          <color theme="1"/>
-          <name val="Century Gothic"/>
-          <family val="2"/>
-          <charset val="162"/>
-          <scheme val="none"/>
-        </font>
-        <alignment horizontal="center" vertical="center" wrapText="1"/>
-      </dxf>
-    </rfmt>
-    <rfmt sheetId="1" sqref="F3" start="0" length="0">
-      <dxf>
-        <font>
-          <sz val="12"/>
-          <color theme="1"/>
-          <name val="Century Gothic"/>
-          <family val="2"/>
-          <charset val="162"/>
-          <scheme val="none"/>
-        </font>
-        <alignment horizontal="center" vertical="center" wrapText="1"/>
-      </dxf>
-    </rfmt>
-    <rfmt sheetId="1" sqref="F4" start="0" length="0">
-      <dxf>
-        <font>
-          <sz val="12"/>
-          <color theme="1"/>
-          <name val="Century Gothic"/>
-          <family val="2"/>
-          <charset val="162"/>
-          <scheme val="none"/>
-        </font>
-        <alignment horizontal="center" vertical="center" wrapText="1"/>
-      </dxf>
-    </rfmt>
-    <rfmt sheetId="1" sqref="F5" start="0" length="0">
-      <dxf>
-        <font>
-          <sz val="12"/>
-          <color theme="1"/>
-          <name val="Century Gothic"/>
-          <family val="2"/>
-          <charset val="162"/>
-          <scheme val="none"/>
-        </font>
-        <alignment horizontal="center" vertical="center" wrapText="1"/>
-      </dxf>
-    </rfmt>
-    <rfmt sheetId="1" sqref="F6" start="0" length="0">
-      <dxf>
-        <font>
-          <sz val="12"/>
-          <color theme="1"/>
-          <name val="Century Gothic"/>
-          <family val="2"/>
-          <charset val="162"/>
-          <scheme val="none"/>
-        </font>
-        <alignment horizontal="center" vertical="center" wrapText="1"/>
-      </dxf>
-    </rfmt>
-    <rfmt sheetId="1" sqref="F7" start="0" length="0">
-      <dxf>
-        <font>
-          <sz val="12"/>
-          <color theme="1"/>
-          <name val="Century Gothic"/>
-          <family val="2"/>
-          <charset val="162"/>
-          <scheme val="none"/>
-        </font>
-        <alignment horizontal="center" vertical="center" wrapText="1"/>
-      </dxf>
-    </rfmt>
-    <rfmt sheetId="1" sqref="F8" start="0" length="0">
-      <dxf>
-        <font>
-          <sz val="12"/>
-          <color theme="1"/>
-          <name val="Century Gothic"/>
-          <family val="2"/>
-          <charset val="162"/>
-          <scheme val="none"/>
-        </font>
-        <alignment horizontal="center" vertical="center" wrapText="1"/>
-      </dxf>
-    </rfmt>
-    <rfmt sheetId="1" sqref="F9" start="0" length="0">
-      <dxf>
-        <font>
-          <sz val="12"/>
-          <color theme="1"/>
-          <name val="Century Gothic"/>
-          <family val="2"/>
-          <charset val="162"/>
-          <scheme val="none"/>
-        </font>
-        <alignment horizontal="center" vertical="center" wrapText="1"/>
-      </dxf>
-    </rfmt>
-    <rfmt sheetId="1" sqref="F10" start="0" length="0">
-      <dxf>
-        <font>
-          <sz val="12"/>
-          <color theme="1"/>
-          <name val="Century Gothic"/>
-          <family val="2"/>
-          <charset val="162"/>
-          <scheme val="none"/>
-        </font>
-        <alignment horizontal="center" vertical="center" wrapText="1"/>
-      </dxf>
-    </rfmt>
-    <rfmt sheetId="1" sqref="F11" start="0" length="0">
-      <dxf>
-        <font>
-          <sz val="12"/>
-          <color theme="1"/>
-          <name val="Century Gothic"/>
-          <family val="2"/>
-          <charset val="162"/>
-          <scheme val="none"/>
-        </font>
-        <alignment horizontal="center" vertical="center" wrapText="1"/>
-      </dxf>
-    </rfmt>
-  </rm>
-  <rrc rId="3" sId="1" ref="D1:D1048576" action="deleteCol">
-    <rfmt sheetId="1" xfDxf="1" sqref="D1:D1048576" start="0" length="0"/>
-  </rrc>
-  <rcc rId="4" sId="1">
-    <oc r="C4">
-      <v>1815</v>
+  <rcc rId="7" sId="1">
+    <oc r="D9">
+      <v>19</v>
     </oc>
-    <nc r="C4" t="inlineStr">
-      <is>
-        <t>15X24X5MM 6802</t>
-      </is>
+    <nc r="D9">
+      <v>21</v>
     </nc>
   </rcc>
-  <rfmt sheetId="1" sqref="A1" start="0" length="0">
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-  </rfmt>
-  <rcc rId="5" sId="1" odxf="1" dxf="1">
-    <oc r="B1" t="inlineStr">
-      <is>
-        <t>SW-File Name(File Name)</t>
-      </is>
-    </oc>
-    <nc r="B1" t="inlineStr">
-      <is>
-        <t>PART</t>
-      </is>
-    </nc>
-    <odxf>
-      <border outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </odxf>
-    <ndxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="1" sqref="C1" start="0" length="0">
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="D1" start="0" length="0">
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-  </rfmt>
-  <rcc rId="6" sId="1">
-    <oc r="B10" t="inlineStr">
-      <is>
-        <r>
-          <t xml:space="preserve">countersunk flat head cross recess </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="SWGDT"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Century Gothic"/>
-            <family val="2"/>
-          </rPr>
-          <t>screw_iso</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="B10" t="inlineStr">
-      <is>
-        <t>countersunk flat head cross recess screw_iso</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="1" sqref="A1:A11" start="0" length="0">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="A1:D1" start="0" length="0">
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="D1:D11" start="0" length="0">
-    <dxf>
-      <border>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="A11:D11" start="0" length="0">
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="A1:D11">
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="A1:A11" start="0" length="0">
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="A1:D1" start="0" length="0">
-    <dxf>
-      <border>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="D1:D11" start="0" length="0">
-    <dxf>
-      <border>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="A11:D11" start="0" length="0">
-    <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="A1:D1" start="0" length="0">
-    <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-  </rfmt>
 </revisions>
 </file>
 
@@ -1344,7 +965,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1491,7 +1112,7 @@
         <v>16</v>
       </c>
       <c r="D9" s="8">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>17</v>

</xml_diff>